<commit_message>
Bug fix - set intent_answer to empty string after collecting the answer.
</commit_message>
<xml_diff>
--- a/contract_flow/CalloutBotDate.xlsx
+++ b/contract_flow/CalloutBotDate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrus/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C370141B-7E86-AF4E-9747-51F7B52FFEB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9394106-8873-E740-9BFD-6514E142F4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="639" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="639" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
@@ -397,10 +397,12 @@
     <t>date</t>
   </si>
   <si>
-    <t>{date}</t>
-  </si>
-  <si>
     <t>What is the date?</t>
+  </si>
+  <si>
+    <t>{date}
+{date} please.
+{date} is preferable.</t>
   </si>
 </sst>
 </file>
@@ -793,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2329718C-D8E4-F44A-A9A8-300068A324E7}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -835,12 +837,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -883,7 +885,7 @@
         <v>118</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -929,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A1AFF7-88CD-41FB-A2D0-6F8B9B7FBC58}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>